<commit_message>
edit the bit numbers of design
</commit_message>
<xml_diff>
--- a/performance.xlsx
+++ b/performance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\333A\Documents\MEGA\Studying\2024-Fall\Digital Comm IC\Final Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9B79E4D6-8960-4109-9EAA-5E7925F17248}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{055456CA-DB33-45AF-B9EA-421A2DF36D1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-105" windowWidth="38640" windowHeight="21240" xr2:uid="{9AF2CF76-7A73-4E71-A441-5E9EBB31A89B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
   <si>
     <t>SNR</t>
   </si>
@@ -42,17 +42,44 @@
     <t>ML_error</t>
   </si>
   <si>
-    <t>VIVADO_error</t>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>500 H matrix</t>
+  </si>
+  <si>
+    <t>1000 H matrix</t>
+  </si>
+  <si>
+    <t>2000 H matrix</t>
+  </si>
+  <si>
+    <t>MATLAB_DFS_L1_floating</t>
+  </si>
+  <si>
+    <t>MATLAB_DFS_L1_fixed</t>
+  </si>
+  <si>
+    <t>VIVADO_DFS_L1_fixed</t>
+  </si>
+  <si>
+    <t>clk_num</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -78,8 +105,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -152,7 +180,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$1</c:f>
+              <c:f>Sheet1!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -187,10 +215,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$10</c:f>
+              <c:f>Sheet1!$A$2:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -217,42 +245,48 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>19</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$10</c:f>
+              <c:f>Sheet1!$B$2:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>3.1469696969696967E-2</c:v>
+                  <c:v>3.1469696969697002E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.840909090909091E-2</c:v>
+                  <c:v>1.8409090909090899E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0121212121212121E-2</c:v>
+                  <c:v>1.01212121212121E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.8333333333333336E-3</c:v>
+                  <c:v>4.8333333333333301E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.0606060606060605E-3</c:v>
+                  <c:v>2.0606060606060601E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.4848484848484851E-4</c:v>
+                  <c:v>8.4848484848484905E-4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.484848484848485E-4</c:v>
+                  <c:v>4.84848484848485E-4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.0606060606060606E-4</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3.0303030303030302E-5</c:v>
+                  <c:v>1.5909090909090899E-4</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.00E+00">
+                  <c:v>5.3030303030302998E-5</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0.00E+00">
+                  <c:v>3.4090909090909099E-5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -260,7 +294,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-1897-4E78-873C-FACC9964E29B}"/>
+              <c16:uniqueId val="{00000000-1A9A-4815-8FC0-64B4432E3AD1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -269,11 +303,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$1</c:f>
+              <c:f>Sheet1!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>VIVADO_error</c:v>
+                  <c:v>MATLAB_DFS_L1_floating</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -304,10 +338,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$10</c:f>
+              <c:f>Sheet1!$A$2:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -334,42 +368,48 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>19</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$10</c:f>
+              <c:f>Sheet1!$C$2:$C$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>3.6439393939393938E-2</c:v>
+                  <c:v>3.6439393939393903E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.3378787878787877E-2</c:v>
+                  <c:v>2.3378787878787902E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.3833333333333333E-2</c:v>
+                  <c:v>1.38333333333333E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.9696969696969695E-3</c:v>
+                  <c:v>6.9696969696969703E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.0303030303030303E-3</c:v>
+                  <c:v>3.0303030303030299E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.6515151515151514E-3</c:v>
+                  <c:v>1.6515151515151499E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.0000000000000001E-4</c:v>
+                  <c:v>7.1969696969696999E-4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.7878787878787879E-4</c:v>
+                  <c:v>3.8636363636363602E-4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.0303030303030302E-5</c:v>
+                  <c:v>1.25E-4</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0.00E+00">
+                  <c:v>7.5757575757575798E-5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -377,7 +417,253 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-1897-4E78-873C-FACC9964E29B}"/>
+              <c16:uniqueId val="{00000001-1A9A-4815-8FC0-64B4432E3AD1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MATLAB_DFS_L1_fixed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>19</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>3.6333333333333301E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.3363636363636399E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.39242424242424E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.7424242424242399E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.04545454545455E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.63636363636364E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.3484848484848501E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.78787878787879E-4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.2121212121212101E-4</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0.00E+00">
+                  <c:v>7.5757575757575798E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-1A9A-4815-8FC0-64B4432E3AD1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>VIVADO_DFS_L1_fixed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>19</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>3.6318181818181798E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.3378787878787902E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.4196969696969699E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.59090909090909E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.0757575757575802E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.46969696969697E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.5757575757575801E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.7121212121212101E-4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.25E-4</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0.00E+00">
+                  <c:v>7.5757575757575798E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-1A9A-4815-8FC0-64B4432E3AD1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -389,11 +675,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1972527952"/>
-        <c:axId val="1972527120"/>
+        <c:axId val="1586961600"/>
+        <c:axId val="1586963680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1972527952"/>
+        <c:axId val="1586961600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -450,12 +736,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1972527120"/>
+        <c:crossAx val="1586963680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1972527120"/>
+        <c:axId val="1586963680"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -513,7 +799,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1972527952"/>
+        <c:crossAx val="1586961600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1160,23 +1446,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>235147</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>89891</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>111670</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>32843</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>178592</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>59531</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>302171</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>98532</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3062D00-C42C-4531-9F0F-24AB94B8FBE9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{320F9DDD-7D69-45F6-A438-C4CAE0145962}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1494,22 +1780,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{580ED746-6353-47D0-99D8-248BBBF9DE11}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.28515625" customWidth="1"/>
-    <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="5" width="26.28515625" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" customWidth="1"/>
+    <col min="7" max="7" width="25.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1517,212 +1805,255 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10</v>
       </c>
       <c r="B2">
-        <v>2077</v>
+        <v>3.1469696969697002E-2</v>
       </c>
       <c r="C2">
-        <v>2405</v>
+        <v>3.6439393939393903E-2</v>
       </c>
       <c r="D2">
-        <f>B2/66000</f>
-        <v>3.1469696969696967E-2</v>
+        <v>3.6333333333333301E-2</v>
       </c>
       <c r="E2">
-        <f>C2/66000</f>
-        <v>3.6439393939393938E-2</v>
+        <v>3.6318181818181798E-2</v>
+      </c>
+      <c r="F2">
+        <v>2670267</v>
+      </c>
+      <c r="G2" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>11</v>
       </c>
       <c r="B3">
-        <v>1215</v>
+        <v>1.8409090909090899E-2</v>
       </c>
       <c r="C3">
-        <v>1543</v>
+        <v>2.3378787878787902E-2</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:E11" si="0">B3/66000</f>
-        <v>1.840909090909091E-2</v>
+        <v>2.3363636363636399E-2</v>
       </c>
       <c r="E3">
-        <f t="shared" si="0"/>
-        <v>2.3378787878787877E-2</v>
+        <v>2.3378787878787902E-2</v>
+      </c>
+      <c r="F3">
+        <v>2607667</v>
+      </c>
+      <c r="G3" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>12</v>
       </c>
       <c r="B4">
-        <v>668</v>
+        <v>1.01212121212121E-2</v>
       </c>
       <c r="C4">
-        <v>913</v>
+        <v>1.38333333333333E-2</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
-        <v>1.0121212121212121E-2</v>
+        <v>1.39242424242424E-2</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
-        <v>1.3833333333333333E-2</v>
+        <v>1.4196969696969699E-2</v>
+      </c>
+      <c r="F4">
+        <v>2556563</v>
+      </c>
+      <c r="G4" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>13</v>
       </c>
       <c r="B5">
-        <v>319</v>
+        <v>4.8333333333333301E-3</v>
       </c>
       <c r="C5">
-        <v>460</v>
+        <v>6.9696969696969703E-3</v>
       </c>
       <c r="D5">
-        <f t="shared" si="0"/>
-        <v>4.8333333333333336E-3</v>
+        <v>6.7424242424242399E-3</v>
       </c>
       <c r="E5">
-        <f t="shared" si="0"/>
-        <v>6.9696969696969695E-3</v>
+        <v>6.59090909090909E-3</v>
+      </c>
+      <c r="F5">
+        <v>2512835</v>
+      </c>
+      <c r="G5" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>14</v>
       </c>
       <c r="B6">
-        <v>136</v>
+        <v>2.0606060606060601E-3</v>
       </c>
       <c r="C6">
-        <v>200</v>
+        <v>3.0303030303030299E-3</v>
       </c>
       <c r="D6">
-        <f t="shared" si="0"/>
-        <v>2.0606060606060605E-3</v>
+        <v>3.04545454545455E-3</v>
       </c>
       <c r="E6">
-        <f t="shared" si="0"/>
-        <v>3.0303030303030303E-3</v>
+        <v>3.0757575757575802E-3</v>
+      </c>
+      <c r="F6">
+        <v>2476227</v>
+      </c>
+      <c r="G6" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>15</v>
       </c>
       <c r="B7">
-        <v>56</v>
+        <v>8.4848484848484905E-4</v>
       </c>
       <c r="C7">
-        <v>109</v>
+        <v>1.6515151515151499E-3</v>
       </c>
       <c r="D7">
-        <f t="shared" si="0"/>
-        <v>8.4848484848484851E-4</v>
+        <v>1.63636363636364E-3</v>
       </c>
       <c r="E7">
-        <f t="shared" si="0"/>
-        <v>1.6515151515151514E-3</v>
+        <v>1.46969696969697E-3</v>
+      </c>
+      <c r="F7">
+        <v>2448563</v>
+      </c>
+      <c r="G7" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>16</v>
       </c>
       <c r="B8">
-        <v>23</v>
+        <v>4.84848484848485E-4</v>
       </c>
       <c r="C8">
-        <v>33</v>
+        <v>7.1969696969696999E-4</v>
       </c>
       <c r="D8">
-        <f t="shared" si="0"/>
-        <v>3.484848484848485E-4</v>
+        <v>7.3484848484848501E-4</v>
       </c>
       <c r="E8">
-        <f t="shared" si="0"/>
-        <v>5.0000000000000001E-4</v>
+        <v>7.5757575757575801E-4</v>
+      </c>
+      <c r="F8">
+        <v>4825587</v>
+      </c>
+      <c r="G8" t="s">
+        <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>17</v>
       </c>
       <c r="B9">
-        <v>7</v>
+        <v>1.5909090909090899E-4</v>
       </c>
       <c r="C9">
-        <v>25</v>
+        <v>3.8636363636363602E-4</v>
       </c>
       <c r="D9">
-        <f t="shared" si="0"/>
-        <v>1.0606060606060606E-4</v>
+        <v>3.78787878787879E-4</v>
       </c>
       <c r="E9">
-        <f t="shared" si="0"/>
-        <v>3.7878787878787879E-4</v>
+        <v>3.7121212121212101E-4</v>
+      </c>
+      <c r="F9">
+        <v>4793795</v>
+      </c>
+      <c r="G9" t="s">
+        <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>18</v>
       </c>
-      <c r="B10">
-        <v>2</v>
+      <c r="B10" s="1">
+        <v>5.3030303030302998E-5</v>
       </c>
       <c r="C10">
-        <v>2</v>
+        <v>1.25E-4</v>
       </c>
       <c r="D10">
-        <f t="shared" si="0"/>
-        <v>3.0303030303030302E-5</v>
+        <v>1.2121212121212101E-4</v>
       </c>
       <c r="E10">
-        <f t="shared" si="0"/>
-        <v>3.0303030303030302E-5</v>
+        <v>1.25E-4</v>
+      </c>
+      <c r="F10">
+        <v>9576947</v>
+      </c>
+      <c r="G10" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>19</v>
       </c>
-      <c r="B11">
-        <v>2</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <f t="shared" si="0"/>
-        <v>3.0303030303030302E-5</v>
-      </c>
-      <c r="E11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>20</v>
+      <c r="B11" s="1">
+        <v>3.4090909090909099E-5</v>
+      </c>
+      <c r="C11" s="1">
+        <v>7.5757575757575798E-5</v>
+      </c>
+      <c r="D11" s="1">
+        <v>7.5757575757575798E-5</v>
+      </c>
+      <c r="E11" s="1">
+        <v>7.5757575757575798E-5</v>
+      </c>
+      <c r="F11" s="1">
+        <v>9541115</v>
+      </c>
+      <c r="G11" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>